<commit_message>
added really basic console input testing
</commit_message>
<xml_diff>
--- a/Armor.xlsx
+++ b/Armor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\source\repos\FalloutFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF44B572-704E-468E-8EA2-48E8E781E6F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8295B0A4-84AC-48D2-9A37-FFD12C4CFB78}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0ECC110E-D7A2-4757-8DA4-CD1DF6A4F133}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0ECC110E-D7A2-4757-8DA4-CD1DF6A4F133}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Environment Suit</t>
   </si>
   <si>
     <t>000c09d4</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>baseid</t>
+  </si>
+  <si>
+    <t>item hp</t>
+  </si>
+  <si>
+    <t>damage rating</t>
+  </si>
+  <si>
+    <t>Chinese Jumpsuit</t>
+  </si>
+  <si>
+    <t>00078646</t>
+  </si>
+  <si>
+    <t>Armored Vault 101 Jumpsuit</t>
+  </si>
+  <si>
+    <t>00034121</t>
+  </si>
+  <si>
+    <t>Child's Vault 101 Jumpsuit</t>
+  </si>
+  <si>
+    <t>000340f2</t>
+  </si>
+  <si>
+    <t>Dad's Wasteland Outfit</t>
+  </si>
+  <si>
+    <t>00079f09</t>
+  </si>
+  <si>
+    <t>Modified Utility Jumpsuit</t>
+  </si>
+  <si>
+    <t>0007c17c</t>
+  </si>
+  <si>
+    <t>Tunnel Snake Outfit</t>
+  </si>
+  <si>
+    <t>0002042e</t>
   </si>
 </sst>
 </file>
@@ -72,8 +126,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,43 +443,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C07C3-D3B4-4179-8694-00150F9ADCBE}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" customWidth="1"/>
     <col min="6" max="6" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>100</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1">
-        <v>2</v>
-      </c>
-      <c r="F1">
-        <v>2</v>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>180</v>
+      </c>
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>100</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some new entries for our Armor.csv file
</commit_message>
<xml_diff>
--- a/Armor.xlsx
+++ b/Armor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AJ\source\repos\FalloutFinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8295B0A4-84AC-48D2-9A37-FFD12C4CFB78}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A71565-CB67-4EC3-B149-39327F6C5F7B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0ECC110E-D7A2-4757-8DA4-CD1DF6A4F133}"/>
+    <workbookView xWindow="19140" yWindow="2325" windowWidth="21600" windowHeight="11385" xr2:uid="{0ECC110E-D7A2-4757-8DA4-CD1DF6A4F133}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Environment Suit</t>
   </si>
@@ -91,6 +91,96 @@
   </si>
   <si>
     <t>0002042e</t>
+  </si>
+  <si>
+    <t>Vault 77 Jumpsuit</t>
+  </si>
+  <si>
+    <t>000cafbe</t>
+  </si>
+  <si>
+    <t>Vault 87 Jumpsuit</t>
+  </si>
+  <si>
+    <t>Vault 92 Jumpsuit</t>
+  </si>
+  <si>
+    <t>Vault 101 Jumpsuit</t>
+  </si>
+  <si>
+    <t>Vault 106 Jumpsuit</t>
+  </si>
+  <si>
+    <t>Vault 108 Jumpsuit</t>
+  </si>
+  <si>
+    <t>Vault 112 Jumpsuit</t>
+  </si>
+  <si>
+    <t>000340ed</t>
+  </si>
+  <si>
+    <t>000b73f3</t>
+  </si>
+  <si>
+    <t>0000431e</t>
+  </si>
+  <si>
+    <t>000b73f2</t>
+  </si>
+  <si>
+    <t>000b73f1</t>
+  </si>
+  <si>
+    <t>000340ef</t>
+  </si>
+  <si>
+    <t>Vault 101 Utility Jumpsuit</t>
+  </si>
+  <si>
+    <t>000425ba</t>
+  </si>
+  <si>
+    <t>Vault 101 Security Armor</t>
+  </si>
+  <si>
+    <t>0003411c</t>
+  </si>
+  <si>
+    <t>Vault Lab Uniform</t>
+  </si>
+  <si>
+    <t>0001cbdc</t>
+  </si>
+  <si>
+    <t>Combat Armor</t>
+  </si>
+  <si>
+    <t>00020420</t>
+  </si>
+  <si>
+    <t>00023030</t>
+  </si>
+  <si>
+    <t>Ranger Battle Armor</t>
+  </si>
+  <si>
+    <t>000239cc</t>
+  </si>
+  <si>
+    <t>Rivet City security uniform</t>
+  </si>
+  <si>
+    <t>Talon Combat Armor</t>
+  </si>
+  <si>
+    <t>000a6f76</t>
+  </si>
+  <si>
+    <t>00034119</t>
+  </si>
+  <si>
+    <t>Tennypenny Security Uniform</t>
   </si>
 </sst>
 </file>
@@ -443,15 +533,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8C07C3-D3B4-4179-8694-00150F9ADCBE}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
@@ -619,6 +709,306 @@
         <v>4</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10">
+        <v>100</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>100</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <v>100</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13">
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14">
+        <v>100</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15">
+        <v>100</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16">
+        <v>100</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>70</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17">
+        <v>100</v>
+      </c>
+      <c r="F17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18">
+        <v>100</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <v>390</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19">
+        <v>400</v>
+      </c>
+      <c r="F19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20">
+        <v>430</v>
+      </c>
+      <c r="C20">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20">
+        <v>1100</v>
+      </c>
+      <c r="F20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21">
+        <v>330</v>
+      </c>
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+      <c r="F21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22">
+        <v>275</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22">
+        <v>300</v>
+      </c>
+      <c r="F22">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23">
+        <v>180</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>